<commit_message>
Refreshed cohort definitions from PL 3.32.0.  Caused some cohortIDs to change.
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2_evan_2.xlsx
+++ b/analysis_specifications/analysis2_evan_2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\HowOften\analysis_specifications\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -10,13 +15,66 @@
     <sheet name="targets" sheetId="1" r:id="rId1"/>
     <sheet name="outcomes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+  <si>
+    <t>cohort_definition_id</t>
+  </si>
+  <si>
+    <t>cohort_definition_name</t>
+  </si>
+  <si>
+    <t>Non-Emergent MNCS (age 18 or greater), post op Afib (any)</t>
+  </si>
+  <si>
+    <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Lower Extremity Bypass - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Carotid Endarterectomy - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Lung Resection - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Esophagectomy - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Pancreatectomy - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Colectomy - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Cystectomy - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Nephrectomy - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
+  </si>
+  <si>
+    <t>clean_window</t>
+  </si>
+  <si>
+    <t>Non-hemorrhagic Stroke</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -110,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +208,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +243,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,143 +419,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>cohort_definition_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>cohort_definition_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>878</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Non-Emergent MNCS (age 18 or greater), post op Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1093</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1094</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Lower Extremity Bypass - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1095</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Carotid Endarterectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1096</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Lung Resection - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+        <v>1268</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1097</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Esophagectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1098</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Pancreatectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1099</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Colectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1100</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cystectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1101</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Nephrectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1102</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1103</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
-        </is>
+      <c r="B13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -496,38 +538,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>cohort_definition_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>cohort_definition_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>clean_window</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1089</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Non-hemorrhagic Stroke</t>
-        </is>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2">
         <v>365</v>

</xml_diff>